<commit_message>
Correct Ensembl ID (human) for AKT2 from ENSG00000142208 to ENSG00000105221 - patch - 1
</commit_message>
<xml_diff>
--- a/cmascore_genes.xlsx
+++ b/cmascore_genes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" state="visible" r:id="rId3"/>
@@ -296,6 +296,9 @@
     <t xml:space="preserve">Akt2</t>
   </si>
   <si>
+    <t xml:space="preserve">ENSG00000105221</t>
+  </si>
+  <si>
     <t xml:space="preserve">ENSMUSG00000004056</t>
   </si>
   <si>
@@ -426,9 +429,6 @@
   </si>
   <si>
     <t xml:space="preserve">ENSMUSG00000037992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENSG00000105221</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -474,6 +474,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -545,64 +551,72 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -857,627 +871,627 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="D7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="D9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="D10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="E12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="I13" s="13" t="s">
         <v>91</v>
       </c>
+      <c r="J13" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="C14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="E14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="G14" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="H14" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="I14" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="J14" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="C15" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="D15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="G15" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="H15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="I15" s="6" t="s">
         <v>106</v>
       </c>
+      <c r="J15" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="A16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="D16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="G16" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="H16" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="I16" s="6" t="s">
         <v>113</v>
       </c>
+      <c r="J16" s="6" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="C17" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="D17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="G17" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="H17" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="I17" s="6" t="s">
         <v>120</v>
       </c>
+      <c r="J17" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="A18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="C18" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="D18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="G18" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="H18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="I18" s="6" t="s">
         <v>127</v>
       </c>
+      <c r="J18" s="6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="A19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="C19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="E19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="G19" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="H19" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="I19" s="6" t="s">
         <v>134</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1498,627 +1512,627 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="D5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="D6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="D7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="D9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="D10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="8" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="1" t="n">
+      <c r="B19" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="I17" s="5" t="s">
+      <c r="E19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct Ensembl ID (mouse) for Hspa8 from ENSMUSG00000024359 to ENSMUSG00000015656
</commit_message>
<xml_diff>
--- a/cmascore_genes.xlsx
+++ b/cmascore_genes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" state="visible" r:id="rId3"/>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">ENSG00000109971</t>
   </si>
   <si>
-    <t xml:space="preserve">ENSMUSG00000024359</t>
+    <t xml:space="preserve">ENSMUSG00000015656</t>
   </si>
   <si>
     <t xml:space="preserve">HSP90AA1</t>
@@ -438,7 +438,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -474,12 +474,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -551,7 +545,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,10 +596,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -871,8 +861,8 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -883,7 +873,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,7 +1285,7 @@
       <c r="H13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="6" t="s">
         <v>91</v>
       </c>
       <c r="J13" s="6" t="s">
@@ -1306,7 +1296,7 @@
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -1402,7 +1392,7 @@
       <c r="A17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>115</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1434,7 +1424,7 @@
       <c r="A18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1512,8 +1502,8 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1524,7 +1514,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1915,7 +1905,7 @@
       <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>115</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1947,7 +1937,7 @@
       <c r="A14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>122</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2075,7 +2065,7 @@
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C18" s="12" t="s">

</xml_diff>